<commit_message>
Feasibility Analysis - ROI calculation
</commit_message>
<xml_diff>
--- a/wiki/Feasibility Analysis.xlsx
+++ b/wiki/Feasibility Analysis.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>Cost Analysis</t>
   </si>
@@ -103,6 +103,24 @@
   </si>
   <si>
     <t>Profit</t>
+  </si>
+  <si>
+    <t>GST @18%</t>
+  </si>
+  <si>
+    <t>Total Fee</t>
+  </si>
+  <si>
+    <t>Deposit</t>
+  </si>
+  <si>
+    <t>Yearly Profit</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>Money Raised</t>
   </si>
 </sst>
 </file>
@@ -134,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -215,20 +233,450 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -241,6 +689,163 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ROI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$39:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>66.691354879114172</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>53.07447319037194</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.261715955864425</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="133294336"/>
+        <c:axId val="133299200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="133294336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="133299200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="133299200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="133294336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,144 +1135,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="38"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="39"/>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="6">
         <v>8000</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="6">
+        <v>20000</v>
+      </c>
+      <c r="D4" s="10">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>12500</v>
+      </c>
+      <c r="C5" s="1">
+        <v>20000</v>
+      </c>
+      <c r="D5" s="12">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1500</v>
+      </c>
+      <c r="D6" s="12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
         <v>12000</v>
       </c>
-      <c r="D4" s="2">
+      <c r="C7" s="1">
         <v>15000</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2">
-        <v>12500</v>
-      </c>
-      <c r="C5" s="2">
-        <v>15000</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="D7" s="12">
         <v>18000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="2">
-        <v>1000</v>
-      </c>
-      <c r="C6" s="2">
-        <v>1500</v>
-      </c>
-      <c r="D6" s="2">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2">
-        <v>12000</v>
-      </c>
-      <c r="C7" s="2">
-        <v>15000</v>
-      </c>
-      <c r="D7" s="2">
-        <v>18000</v>
-      </c>
-    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>4000</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>6000</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="12">
         <v>6000</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>6000</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>8000</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="12">
         <v>10000</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <f>SUM(B4:B9)</f>
         <v>43500</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <f>SUM(C4:C9)</f>
-        <v>57500</v>
-      </c>
-      <c r="D10" s="2">
+        <v>70500</v>
+      </c>
+      <c r="D10" s="12">
         <f>SUM(D4:D9)</f>
         <v>69000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="2">
@@ -676,301 +1290,408 @@
       <c r="C11" s="2">
         <v>30</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="14">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="2">
-        <f>B10/B11</f>
-        <v>1450</v>
-      </c>
-      <c r="C12" s="2">
-        <f>C10/40</f>
-        <v>1437.5</v>
-      </c>
-      <c r="D12" s="2">
-        <f>D10/D11</f>
-        <v>2300</v>
+      <c r="B12" s="41">
+        <f>-B10/B11</f>
+        <v>-1450</v>
+      </c>
+      <c r="C12" s="41">
+        <f>-C10/40</f>
+        <v>-1762.5</v>
+      </c>
+      <c r="D12" s="42">
+        <f>-D10/D11</f>
+        <v>-2300</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="48"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="20">
+        <v>200000</v>
+      </c>
+      <c r="C14" s="20">
+        <v>400000</v>
+      </c>
+      <c r="D14" s="25">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="49"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="19"/>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B16" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C16" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D16" s="45" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="15">
+        <v>50000</v>
+      </c>
+      <c r="C17" s="15">
+        <v>60000</v>
+      </c>
+      <c r="D17" s="30">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B18" s="6">
         <v>60000</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C18" s="6">
         <v>75000</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D18" s="10">
         <v>100000</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B19" s="1">
         <v>350000</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C19" s="1">
         <v>400000</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D19" s="12">
         <v>550000</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B20" s="1">
         <v>50000</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C20" s="1">
         <v>60000</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D20" s="12">
         <v>75000</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B21" s="1">
         <v>50000</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C21" s="1">
         <v>65000</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D21" s="12">
         <v>80000</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B22" s="1">
         <v>5000</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C22" s="1">
         <v>8000</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D22" s="12">
         <v>10000</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B23" s="1">
         <v>5000</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C23" s="1">
         <v>7000</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D23" s="12">
         <v>9000</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B24" s="1">
         <v>8000</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C24" s="1">
         <v>1000</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D24" s="12">
         <v>12000</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="2">
-        <f>SUM(B15:B21)</f>
-        <v>528000</v>
-      </c>
-      <c r="C22" s="2">
-        <f>SUM(C15:C21)</f>
-        <v>616000</v>
-      </c>
-      <c r="D22" s="2">
-        <f>SUM(D15:D21)</f>
-        <v>836000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="B25" s="1">
+        <f>SUM(B17:B24)</f>
+        <v>578000</v>
+      </c>
+      <c r="C25" s="1">
+        <f>SUM(C17:C24)</f>
+        <v>676000</v>
+      </c>
+      <c r="D25" s="12">
+        <f>SUM(D17:D24)</f>
+        <v>911000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B26" s="1">
         <v>11.3</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C26" s="1">
         <v>13</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D26" s="12">
         <v>14.5</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B27" s="1">
         <v>60</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C27" s="1">
         <v>60</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D27" s="12">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2">
-        <v>11560</v>
-      </c>
-      <c r="C25" s="2">
-        <v>14016</v>
-      </c>
-      <c r="D25" s="2">
-        <v>18800</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="B28" s="17">
+        <f>PMT(11.3%/12,5*12,B25-B14)</f>
+        <v>-8275.3024846391072</v>
+      </c>
+      <c r="C28" s="17">
+        <f>PMT(12.5%/12,60,C25-C14)</f>
+        <v>-6209.4309502147717</v>
+      </c>
+      <c r="D28" s="31">
+        <f>PMT(13%/12,60,D25-D14)</f>
+        <v>-19590.395891076882</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B29" s="1">
         <v>30</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C29" s="1">
         <v>30</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D29" s="12">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="B27" s="2">
-        <f>B25/B26</f>
-        <v>385.33333333333331</v>
-      </c>
-      <c r="C27" s="2">
-        <f>C25/C26</f>
-        <v>467.2</v>
-      </c>
-      <c r="D27" s="2">
-        <f>D25/D26</f>
-        <v>626.66666666666663</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B30" s="27">
+        <f>B28/B29</f>
+        <v>-275.84341615463688</v>
+      </c>
+      <c r="C30" s="27">
+        <f>C28/C29</f>
+        <v>-206.98103167382573</v>
+      </c>
+      <c r="D30" s="28">
+        <f>D28/D29</f>
+        <v>-653.01319636922938</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B29" s="2">
-        <f>B12+B27</f>
-        <v>1835.3333333333333</v>
-      </c>
-      <c r="C29" s="2">
-        <f>C12+C27</f>
-        <v>1904.7</v>
-      </c>
-      <c r="D29" s="2">
-        <f>D12+D27</f>
-        <v>2926.6666666666665</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="B32" s="1">
+        <f>B12+B30</f>
+        <v>-1725.843416154637</v>
+      </c>
+      <c r="C32" s="1">
+        <f>C12+C30</f>
+        <v>-1969.4810316738258</v>
+      </c>
+      <c r="D32" s="1">
+        <f>D12+D30</f>
+        <v>-2953.0131963692293</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B34" s="2">
+        <f>B36-B35</f>
+        <v>2796.6101694915255</v>
+      </c>
+      <c r="C34" s="2">
+        <f>C36-C35</f>
+        <v>2966.1016949152545</v>
+      </c>
+      <c r="D34" s="2">
+        <f>D36-D35</f>
+        <v>3389.8305084745762</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="15">
+        <f>(B36/1.18)*0.18</f>
+        <v>503.38983050847457</v>
+      </c>
+      <c r="C35" s="15">
+        <f>(C36/1.18)*0.18</f>
+        <v>533.89830508474574</v>
+      </c>
+      <c r="D35" s="7">
+        <f>(D36/1.18)*0.18</f>
+        <v>610.16949152542372</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36" s="15">
         <v>3300</v>
       </c>
-      <c r="C31" s="3">
-        <v>3000</v>
-      </c>
-      <c r="D31" s="3">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="C36" s="15">
+        <v>3500</v>
+      </c>
+      <c r="D36" s="7">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="5">
-        <f>(B31-B29)*B26</f>
-        <v>43940</v>
-      </c>
-      <c r="C32" s="5">
-        <f>(C31-C29)*C26</f>
-        <v>32859</v>
-      </c>
-      <c r="D32" s="6">
-        <f>(D31-D29)*D26</f>
-        <v>38200.000000000007</v>
+      <c r="B37" s="22">
+        <f>(B34+B32)*B29</f>
+        <v>32123.002600106658</v>
+      </c>
+      <c r="C37" s="22">
+        <f>(C34+C32)*C29</f>
+        <v>29898.619897242861</v>
+      </c>
+      <c r="D37" s="23">
+        <f>(D34+D32)*D29</f>
+        <v>13104.519363160407</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="20">
+        <f>B37*12</f>
+        <v>385476.0312012799</v>
+      </c>
+      <c r="C38" s="20">
+        <f>C37*12</f>
+        <v>358783.4387669143</v>
+      </c>
+      <c r="D38" s="25">
+        <f>D37*12</f>
+        <v>157254.23235792489</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" s="27">
+        <f>B38/B25*100</f>
+        <v>66.691354879114172</v>
+      </c>
+      <c r="C39" s="27">
+        <f>C38*100/C25</f>
+        <v>53.07447319037194</v>
+      </c>
+      <c r="D39" s="28">
+        <f>D38/D25*100</f>
+        <v>17.261715955864425</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>